<commit_message>
refreshed logistic reg with kfolds
</commit_message>
<xml_diff>
--- a/Report/Accuracies_Logistic_Regression_Nikita.xlsx
+++ b/Report/Accuracies_Logistic_Regression_Nikita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Никита\UNI\Master\4.Semester\KIinPE\Project\Predictive-Quality-Battery-TUM\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B44984-AEDB-417E-BBC3-736A20C04357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA97605-E5D0-43B9-A5E7-584D9F204E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9270" yWindow="4215" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>0.822</t>
   </si>
   <si>
-    <t>0.910</t>
-  </si>
-  <si>
     <t>0.812</t>
   </si>
   <si>
@@ -91,10 +88,15 @@
     <t>0.696</t>
   </si>
   <si>
-    <t>0.670</t>
-  </si>
-  <si>
     <t>No vlaues since RAW data performed best</t>
+  </si>
+  <si>
+    <t>0.652
+false pos. 44, false n. 0</t>
+  </si>
+  <si>
+    <t>0.903
+false pos. 2 false n. 10</t>
   </si>
 </sst>
 </file>
@@ -286,11 +288,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -332,6 +333,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,107 +621,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F8"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added false negatives to accuracies.xlsx, finalised log reg .py
</commit_message>
<xml_diff>
--- a/Report/Accuracies_Logistic_Regression_Nikita.xlsx
+++ b/Report/Accuracies_Logistic_Regression_Nikita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Никита\UNI\Master\4.Semester\KIinPE\Project\Predictive-Quality-Battery-TUM\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA97605-E5D0-43B9-A5E7-584D9F204E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B3D170-3259-486B-B09C-818F0923C29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9270" yWindow="4215" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7410" yWindow="3795" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>x</t>
   </si>
@@ -68,35 +68,50 @@
   </si>
   <si>
     <t>Schmierstoff vorhanden</t>
-  </si>
-  <si>
-    <t>0.785</t>
-  </si>
-  <si>
-    <t>0.822</t>
-  </si>
-  <si>
-    <t>0.812</t>
-  </si>
-  <si>
-    <t>0.831</t>
-  </si>
-  <si>
-    <t>0.668</t>
-  </si>
-  <si>
-    <t>0.696</t>
-  </si>
-  <si>
-    <t>No vlaues since RAW data performed best</t>
-  </si>
-  <si>
-    <t>0.652
-false pos. 44, false n. 0</t>
   </si>
   <si>
     <t>0.903
 false pos. 2 false n. 10</t>
+  </si>
+  <si>
+    <t>0.798
+false pos. 0 false n. 26</t>
+  </si>
+  <si>
+    <t>0.823
+false pos. 0 false n. 22</t>
+  </si>
+  <si>
+    <t>0.8358
+false pos. 0 false n. 21</t>
+  </si>
+  <si>
+    <t>0.838
+false pos. 0 false n. 21</t>
+  </si>
+  <si>
+    <t>0.659
+false pos. 0 false n. 43</t>
+  </si>
+  <si>
+    <t>0.653
+false pos. 44 false n. 0</t>
+  </si>
+  <si>
+    <t>0.653 
+false pos. 44 false n. 0</t>
+  </si>
+  <si>
+    <t>0.653
+false pos. 44, false n. 0</t>
+  </si>
+  <si>
+    <t>0.690
+false pos. 1 false n. 39</t>
+  </si>
+  <si>
+    <t>0.697
+false pos. 1 false n. 37</t>
   </si>
 </sst>
 </file>
@@ -120,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -155,26 +170,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -193,17 +188,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -288,59 +272,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +590,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,99 +602,120 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
+      <c r="C6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
+      <c r="C8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="21"/>
+      <c r="C12" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D5:F8"/>
+  <mergeCells count="1">
     <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final Accuracies log Reg
</commit_message>
<xml_diff>
--- a/Report/Accuracies_Logistic_Regression_Nikita.xlsx
+++ b/Report/Accuracies_Logistic_Regression_Nikita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Никита\UNI\Master\4.Semester\KIinPE\Project\Predictive-Quality-Battery-TUM\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B3D170-3259-486B-B09C-818F0923C29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85287664-93D0-4621-A916-6FD1E527D06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="3795" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3795" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -70,48 +70,56 @@
     <t>Schmierstoff vorhanden</t>
   </si>
   <si>
-    <t>0.903
+    <t>0.903 +-0.023
 false pos. 2 false n. 10</t>
   </si>
   <si>
-    <t>0.798
+    <t>0.823 +-0.017
+false pos. 0 false n. 22</t>
+  </si>
+  <si>
+    <t>0.798 +-0.008
 false pos. 0 false n. 26</t>
   </si>
   <si>
-    <t>0.823
-false pos. 0 false n. 22</t>
-  </si>
-  <si>
-    <t>0.8358
+    <t>0.8358 +-0.016
 false pos. 0 false n. 21</t>
   </si>
   <si>
-    <t>0.838
+    <t>0.659 +-0.005
+false pos. 0 false n. 43</t>
+  </si>
+  <si>
+    <t>0.659 +-0.003
+false pos. 0 false n. 43</t>
+  </si>
+  <si>
+    <t>0.659 +- 0.003
+false pos. 0 false n. 43</t>
+  </si>
+  <si>
+    <t>0.697 +-0.015
+false pos. 1 false n. 37</t>
+  </si>
+  <si>
+    <t>0.697 +- 0.014
+false pos. 1 false n. 37</t>
+  </si>
+  <si>
+    <t>0.690 +- 0.014
+false pos. 1 false n. 39</t>
+  </si>
+  <si>
+    <t>0.653 +-0.002
+false pos. 44, false n. 0</t>
+  </si>
+  <si>
+    <t>0.653 +-0.002
+false pos. 44 false n. 0</t>
+  </si>
+  <si>
+    <t>0.838 +- 0.015
 false pos. 0 false n. 21</t>
-  </si>
-  <si>
-    <t>0.659
-false pos. 0 false n. 43</t>
-  </si>
-  <si>
-    <t>0.653
-false pos. 44 false n. 0</t>
-  </si>
-  <si>
-    <t>0.653 
-false pos. 44 false n. 0</t>
-  </si>
-  <si>
-    <t>0.653
-false pos. 44, false n. 0</t>
-  </si>
-  <si>
-    <t>0.690
-false pos. 1 false n. 39</t>
-  </si>
-  <si>
-    <t>0.697
-false pos. 1 false n. 37</t>
   </si>
 </sst>
 </file>
@@ -281,15 +289,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -307,6 +306,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +598,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,18 +610,18 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -630,85 +638,85 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>18</v>
+      <c r="E5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="14" t="s">
+      <c r="C6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>17</v>
+      <c r="F6" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>17</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="C8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>